<commit_message>
XLSX - Adjust initial width for columns based on values
</commit_message>
<xml_diff>
--- a/dist/xlsx/world_countries.xlsx
+++ b/dist/xlsx/world_countries.xlsx
@@ -432,6 +432,16 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="6" customWidth="1" min="2" max="2"/>
+    <col width="6" customWidth="1" min="3" max="3"/>
+    <col width="44" customWidth="1" min="4" max="4"/>
+    <col width="49" customWidth="1" min="5" max="5"/>
+    <col width="41" customWidth="1" min="6" max="6"/>
+    <col width="44" customWidth="1" min="7" max="7"/>
+    <col width="42" customWidth="1" min="8" max="8"/>
+    <col width="3" customWidth="1" min="9" max="9"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">

</xml_diff>